<commit_message>
data through 2018 and edited methods
</commit_message>
<xml_diff>
--- a/nes-lter-picoeuk-mvco-info.xlsx
+++ b/nes-lter-picoeuk-mvco-info.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\WHOIGit\nes-lter-picoeuk-mvco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
   <si>
     <t>keyword</t>
   </si>
@@ -193,9 +193,6 @@
     <t>depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>abundance_picoeuk</t>
-  </si>
-  <si>
     <t>NODC Data Types Thesaurus</t>
   </si>
   <si>
@@ -241,10 +238,52 @@
     <t>SeaVoX water bodies</t>
   </si>
   <si>
-    <t>number of eukaryote picophytoplankton cells per milliliter of the water body http://vocab.nerc.ac.uk/collection/P01/current/SDBIOL01/ http://vocab.nerc.ac.uk/collection/F02/current/F0200004/</t>
-  </si>
-  <si>
     <t>numberPerMilliliter</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Olson</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Woods Hole Oceanographic Institution</t>
+  </si>
+  <si>
+    <t>E. Taylor</t>
+  </si>
+  <si>
+    <t>Crockford</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>technician</t>
+  </si>
+  <si>
+    <t>Alexi</t>
+  </si>
+  <si>
+    <t>Shalapyonok</t>
+  </si>
+  <si>
+    <t>ashalapyonok@whoi.edu</t>
+  </si>
+  <si>
+    <t>metadataProvider</t>
+  </si>
+  <si>
+    <t>concentration_picoeuk</t>
+  </si>
+  <si>
+    <t>abundance per unit volume of eukaryote picophytoplankton http://vocab.nerc.ac.uk/collection/P01/current/SDBIOL01/ http://vocab.nerc.ac.uk/collection/F02/current/F0200004/</t>
+  </si>
+  <si>
+    <t>rolson@whoi.edu</t>
   </si>
 </sst>
 </file>
@@ -567,7 +606,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,16 +639,16 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>40</v>
@@ -705,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,16 +789,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
@@ -776,34 +821,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -826,6 +859,84 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -838,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -889,7 +1000,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -897,18 +1008,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -916,55 +1027,55 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
         <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated abstract, methods, personnel
</commit_message>
<xml_diff>
--- a/nes-lter-picoeuk-mvco-info.xlsx
+++ b/nes-lter-picoeuk-mvco-info.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t>keyword</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>rolson@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0001-8655-7253</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,6 +929,9 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>86</v>
       </c>
       <c r="G7" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
edited methods, added copy of data file with space replacing T delimiter
</commit_message>
<xml_diff>
--- a/nes-lter-picoeuk-mvco-info.xlsx
+++ b/nes-lter-picoeuk-mvco-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="5" r:id="rId1"/>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,18 +640,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>84</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>40</v>
@@ -660,18 +660,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
@@ -749,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>